<commit_message>
Updated sql design document with all table creation queries
</commit_message>
<xml_diff>
--- a/SQL/DatabaseDesign.xlsx
+++ b/SQL/DatabaseDesign.xlsx
@@ -20,11 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t xml:space="preserve">APP_INSTANCE_DATA</t>
   </si>
   <si>
+    <t xml:space="preserve">create table APP_INSTANCE_DATA
+(
+     APP_ID SERIAL PRIMARY KEY,
+     APP_NAME CHARACTER VARYING(255) NOT NULL,
+     APP_TYPE CHARACTER VARYING(255) NOT NULL
+);</t>
+  </si>
+  <si>
     <t xml:space="preserve">APP_ID</t>
   </si>
   <si>
@@ -37,18 +45,42 @@
     <t xml:space="preserve">APP_INSTANCE_PAYLOAD</t>
   </si>
   <si>
+    <t xml:space="preserve">create table APP_INSTANCE_PAYLOAD
+(   
+    APP_ID INTEGER NOT NULL,
+    PAYLOAD BYTEA NOT NULL
+);
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAYLOAD</t>
   </si>
   <si>
     <t xml:space="preserve">TEAM_APPS</t>
   </si>
   <si>
+    <t xml:space="preserve">create table TEAM_APPS
+(
+APP_ID INTEGER NOT NULL,
+TEAM_ID INTEGER NOT NULL
+);
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEAM_ID</t>
   </si>
   <si>
     <t xml:space="preserve">TEAMS</t>
   </si>
   <si>
+    <t xml:space="preserve">create table TEAMS
+(
+    TEAM_ID INTEGER NOT NULL,
+    TEAM_NAME CHARACTER VARYING(255) NOT NULL,
+    TEAM_DL CHARACTER VARYING(255) NOT NULL
+);</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEAM_NAME</t>
   </si>
   <si>
@@ -58,13 +90,35 @@
     <t xml:space="preserve">USER_TEAM_RELATION</t>
   </si>
   <si>
+    <t xml:space="preserve">
+create table USER_TEAM_RELATION
+(
+USER_ID INTEGER NOT NULL,
+TEAM_ID INTEGER NOT NULL
+);
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">USER_ID</t>
   </si>
   <si>
     <t xml:space="preserve">PERSONAL_APPS</t>
   </si>
   <si>
+    <t xml:space="preserve">create table PERSONAL_APPS
+(
+USER_ID INTEGER NOT NULL,
+APP_ID INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLOBAL_APPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create table GLOBAL_APPS
+(
+APP_ID INTEGER NOT NULL
+);</t>
   </si>
 </sst>
 </file>
@@ -79,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,13 +199,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -174,145 +233,167 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>1</v>
+      <c r="A29" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2"/>
+      <c r="A34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2"/>
+      <c r="A35" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Created entity and repository according to database design
</commit_message>
<xml_diff>
--- a/SQL/DatabaseDesign.xlsx
+++ b/SQL/DatabaseDesign.xlsx
@@ -20,20 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t xml:space="preserve">APP_INSTANCE_DATA</t>
   </si>
   <si>
     <t xml:space="preserve">create table APP_INSTANCE_DATA
 (
-     APP_ID SERIAL PRIMARY KEY,
-     APP_NAME CHARACTER VARYING(255) NOT NULL,
-     APP_TYPE CHARACTER VARYING(255) NOT NULL
-);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APP_ID</t>
+     ID SERIAL PRIMARY KEY,
+     NAME CHARACTER VARYING(255) NOT NULL,
+     TYPE CHARACTER VARYING(255) NOT NULL
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">NAME</t>
@@ -47,10 +47,13 @@
   <si>
     <t xml:space="preserve">create table APP_INSTANCE_PAYLOAD
 (   
-    APP_ID INTEGER NOT NULL,
+     ID SERIAL PRIMARY KEY,
+     APP_ID INTEGER NOT NULL UNIQUE,
     PAYLOAD BYTEA NOT NULL
-);
-</t>
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APP_ID</t>
   </si>
   <si>
     <t xml:space="preserve">PAYLOAD</t>
@@ -61,10 +64,10 @@
   <si>
     <t xml:space="preserve">create table TEAM_APPS
 (
-APP_ID INTEGER NOT NULL,
-TEAM_ID INTEGER NOT NULL
-);
-</t>
+    ID SERIAL PRIMARY KEY,
+    APP_ID INTEGER NOT NULL,
+    TEAM_ID INTEGER NOT NULL
+);</t>
   </si>
   <si>
     <t xml:space="preserve">TEAM_ID</t>
@@ -73,12 +76,37 @@
     <t xml:space="preserve">TEAMS</t>
   </si>
   <si>
-    <t xml:space="preserve">create table TEAMS
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">create table TEAMS
 (
-    TEAM_ID INTEGER NOT NULL,
-    TEAM_NAME CHARACTER VARYING(255) NOT NULL,
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    TEAM_NAME CHARACTER VARYING(255) NOT NULL,
     TEAM_DL CHARACTER VARYING(255) NOT NULL
 );</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TEAM_NAME</t>
@@ -90,13 +118,38 @@
     <t xml:space="preserve">USER_TEAM_RELATION</t>
   </si>
   <si>
-    <t xml:space="preserve">
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
 create table USER_TEAM_RELATION
 (
-USER_ID INTEGER NOT NULL,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">USER_ID INTEGER NOT NULL,
 TEAM_ID INTEGER NOT NULL
-);
-</t>
+);</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">USER_ID</t>
@@ -105,20 +158,72 @@
     <t xml:space="preserve">PERSONAL_APPS</t>
   </si>
   <si>
-    <t xml:space="preserve">create table PERSONAL_APPS
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">create table PERSONAL_APPS
 (
-USER_ID INTEGER NOT NULL,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">USER_ID INTEGER NOT NULL,
 APP_ID INTEGER NOT NULL
 );</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">GLOBAL_APPS</t>
   </si>
   <si>
-    <t xml:space="preserve">create table GLOBAL_APPS
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">create table GLOBAL_APPS
 (
-APP_ID INTEGER NOT NULL
-);</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">APP_ID INTEGER NOT NULL
+);</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -128,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -149,6 +254,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +323,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,16 +355,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -277,123 +399,153 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>2</v>
-      </c>
+    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>2</v>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="23" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="28" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added context menu option table sql
</commit_message>
<xml_diff>
--- a/SQL/DatabaseDesign.xlsx
+++ b/SQL/DatabaseDesign.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t xml:space="preserve">APP_INSTANCE_DATA</t>
   </si>
@@ -74,6 +74,59 @@
   </si>
   <si>
     <t xml:space="preserve">TEAMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create table TEAMS
+(
+   ID SERIAL PRIMARY KEY,
+    TEAM_NAME CHARACTER VARYING(255) NOT NULL,
+    TEAM_DL CHARACTER VARYING(255) NOT NULL
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM_DL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_TEAM_RELATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+create table USER_TEAM_RELATION
+(
+ID SERIAL PRIMARY KEY,
+USER_ID INTEGER NOT NULL,
+TEAM_ID INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERSONAL_APPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create table PERSONAL_APPS
+(
+ID SERIAL PRIMARY KEY,
+USER_ID INTEGER NOT NULL,
+APP_ID INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLOBAL_APPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create table GLOBAL_APPS
+(
+ID SERIAL PRIMARY KEY,
+APP_ID INTEGER NOT NULL
+);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTEXT_MENU_OPTIONS</t>
   </si>
   <si>
     <r>
@@ -83,9 +136,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">create table TEAMS
-(
-   </t>
+      <t xml:space="preserve">create table </t>
     </r>
     <r>
       <rPr>
@@ -93,7 +144,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+      <t xml:space="preserve">CONTEXT_MENU_OPTIONS
 </t>
     </r>
     <r>
@@ -103,31 +154,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">    TEAM_NAME CHARACTER VARYING(255) NOT NULL,
-    TEAM_DL CHARACTER VARYING(255) NOT NULL
-);</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM_DL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USER_TEAM_RELATION</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-create table USER_TEAM_RELATION
-(
+      <t xml:space="preserve">(
+ID SERIAL PRIMARY KEY,
 </t>
     </r>
     <r>
@@ -136,7 +164,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
+      <t xml:space="preserve">TYPE CHARACTER VARYING(255) NOT NULL,
+OPTION_LIST CHARACTER VARYING(255) NOT NULL
 </t>
     </r>
     <r>
@@ -146,84 +175,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">USER_ID INTEGER NOT NULL,
-TEAM_ID INTEGER NOT NULL
-);</t>
+      <t xml:space="preserve">);</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">USER_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PERSONAL_APPS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">create table PERSONAL_APPS
-(
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">USER_ID INTEGER NOT NULL,
-APP_ID INTEGER NOT NULL
-);</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">GLOBAL_APPS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">create table GLOBAL_APPS
-(
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ID SERIAL PRIMARY KEY,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">APP_ID INTEGER NOT NULL
-);</t>
-    </r>
+    <t xml:space="preserve">OPTION_LIST</t>
   </si>
 </sst>
 </file>
@@ -309,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,15 +282,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,8 +305,8 @@
   </sheetPr>
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -399,11 +347,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -424,7 +372,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2"/>
@@ -470,11 +418,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="5"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -494,11 +442,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="5"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -518,11 +466,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="5"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
@@ -532,17 +480,29 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
+    <row r="36" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
+      <c r="A37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3"/>
+      <c r="A38" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3"/>
+      <c r="A39" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>

</xml_diff>